<commit_message>
teste de extração e planilha
</commit_message>
<xml_diff>
--- a/docs/planilha_produtos.xlsx
+++ b/docs/planilha_produtos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
   <si>
     <t xml:space="preserve">CODPRO</t>
   </si>
@@ -49,7 +49,7 @@
     <t xml:space="preserve">CERTIFICADOS_HTML</t>
   </si>
   <si>
-    <t xml:space="preserve">Categoria_do_produto_pesquisado</t>
+    <t xml:space="preserve">CATEGORIA_PRODUTO</t>
   </si>
 </sst>
 </file>
@@ -59,7 +59,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,13 +89,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -147,20 +140,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -358,56 +355,56 @@
   </sheetPr>
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="27.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="23.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="34.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="73.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="8.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="27.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="19.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="23.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="19.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="34.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="73.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="1" width="8.95"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="K1" s="2" t="s">
@@ -416,11 +413,84 @@
       <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="3"/>
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="F3" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="I3" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="K3" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="L3" s="4" t="n">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
método para verificar próxima linha a ser preenchida
</commit_message>
<xml_diff>
--- a/docs/planilha_produtos.xlsx
+++ b/docs/planilha_produtos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
     <t xml:space="preserve">CODPRO</t>
   </si>
@@ -50,6 +50,36 @@
   </si>
   <si>
     <t xml:space="preserve">CATEGORIA_PRODUTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conteúdo da Embalagem:  1 Luva de lã sintética.  Resistente e prática, não risca e nem danifica a lataria do veículo. Contém punho de algodão para melhor fixação na mão do operador.  Indicada para polimento de superfícies, proporcionando ótimo acabamento e brilho. Ideal para uso automotivo. Atenção: o produto não risca a superfície, mas pode reter resíduos que riscam. Certifique-se de que a luva esteja limpa e livre de resíduos antes de usá-la.  Garantia legal: 90 dias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.vonder.com.br/produto/luva_de_l_sinttica_para_polimento_vonder/4468</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luva de lã sintética para polimento VONDER 63.64.025.019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;div class="descricaoProd"&gt;
+               &lt;b&gt;Conteúdo da Embalagem:&lt;/b&gt; &lt;br&gt;                     
+                      &lt;p style="margin-left: 5px; padding-bottom: 10px;"&gt;1 Luva de lã sintética.&lt;/p&gt;&lt;br&gt;
+                      &lt;p style="margin-left: 5px; padding-bottom: 10px;"&gt;Resistente e prática, não risca e nem danifica a lataria do veículo. Contém punho de algodão para melhor fixação na mão do operador.&lt;/p&gt;&lt;br&gt;
+                      &lt;p style="margin-left: 5px; padding-bottom: 10px;"&gt;Indicada para polimento de superfícies, proporcionando ótimo acabamento e brilho. Ideal para uso automotivo. Atenção: o produto não risca a superfície, mas pode reter resíduos que riscam. Certifique-se de que a luva esteja limpa e livre de resíduos antes de usá-la.&lt;/p&gt;&lt;br&gt;
+                      &lt;p style="margin-left: 5px; padding-bottom: 10px;"&gt;Garantia legal: 90 dias&lt;/p&gt;&lt;br&gt;
+                            &lt;div class="arquivoItens"&gt; 
+                                       &lt;/div&gt;
+            &lt;/div&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comprimento: 250 mm
+Largura: 190 mm
+Material: Lã sintética (100% Poliester)
+Punho: Algodão
+Massa aproximada (peso): 0,1 kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Equipamentos de proteção individual, coletiva, sinalização e segurança| Equipamentos para proteção de braços e mãos</t>
   </si>
 </sst>
 </file>
@@ -59,7 +89,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,13 +119,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -154,36 +177,32 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -382,27 +401,27 @@
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="2:2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="296.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="33.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="27.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="19.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="23.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="296.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="132.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="296.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="109.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="19.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="34.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="73.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="1" width="8.95"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -415,7 +434,7 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -436,30 +455,69 @@
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="n">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="n">
         <v>6364025019</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
+      <c r="B2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6"/>
-      <c r="C3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="L3" s="7"/>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="n">
+        <v>6364025019</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" s="5"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6"/>
     </row>
   </sheetData>

</xml_diff>